<commit_message>
Processed P vs I data, updated alpha and pmax
</commit_message>
<xml_diff>
--- a/Data_processed/CM_F16.xlsx
+++ b/Data_processed/CM_F16.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PikesStuff/Desktop/Tris_Data/Carmel_Bay_Fall_2016/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PikesStuff/github/McHugh-et-al/Data_processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CF17C-1944-8546-994F-B8A57AF464C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456DB0FC-CBCD-384A-990B-376909C79BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28720" yWindow="-1360" windowWidth="15400" windowHeight="14000" xr2:uid="{269C1F22-356E-CF4D-AA30-B493EC9AF6CA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="4" xr2:uid="{269C1F22-356E-CF4D-AA30-B493EC9AF6CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Calliarthron" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="12">
   <si>
     <t>PAR</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Thinwire</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>pmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pmax </t>
   </si>
 </sst>
 </file>
@@ -91,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B30990A-EC2E-5F4A-987F-88FE498752D8}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,8 +438,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -442,8 +458,14 @@
       <c r="D2">
         <v>-4.5208333333333332E-5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F2">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -456,8 +478,14 @@
       <c r="D3">
         <v>-2.9583333333333335E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F3">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -470,8 +498,14 @@
       <c r="D4">
         <v>-2.7291666666666672E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F4">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -484,8 +518,14 @@
       <c r="D5">
         <v>-1.3958333333333335E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F5">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>30</v>
       </c>
@@ -498,8 +538,14 @@
       <c r="D6">
         <v>-6.8750000000000011E-6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F6">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>40</v>
       </c>
@@ -512,8 +558,14 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F7">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>62</v>
       </c>
@@ -526,8 +578,14 @@
       <c r="D8">
         <v>8.7499999999999992E-6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F8">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>116</v>
       </c>
@@ -540,8 +598,14 @@
       <c r="D9">
         <v>3.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F9">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -554,8 +618,14 @@
       <c r="D10">
         <v>-3.2093023255813954E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F10">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -568,8 +638,14 @@
       <c r="D11">
         <v>-7.4418604651162789E-6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F11">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -582,8 +658,14 @@
       <c r="D12">
         <v>1.3953488372093025E-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F12">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>8</v>
       </c>
@@ -596,8 +678,14 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F13">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>30</v>
       </c>
@@ -610,8 +698,14 @@
       <c r="D14">
         <v>1.4186046511627907E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>40</v>
       </c>
@@ -624,8 +718,14 @@
       <c r="D15">
         <v>6.511627906976744E-6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F15">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>62</v>
       </c>
@@ -638,8 +738,14 @@
       <c r="D16">
         <v>3.1860465116279072E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F16">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>116</v>
       </c>
@@ -652,8 +758,14 @@
       <c r="D17">
         <v>1.5651162790697676E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F17">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>0</v>
       </c>
@@ -666,8 +778,14 @@
       <c r="D18">
         <v>-1.3448275862068966E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2</v>
       </c>
@@ -680,8 +798,14 @@
       <c r="D19">
         <v>-1.5517241379310346E-6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -694,8 +818,14 @@
       <c r="D20">
         <v>-6.8965517241379312E-7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>8</v>
       </c>
@@ -708,8 +838,14 @@
       <c r="D21">
         <v>4.8275862068965517E-6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30</v>
       </c>
@@ -722,8 +858,14 @@
       <c r="D22">
         <v>-4.8275862068965517E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>40</v>
       </c>
@@ -736,8 +878,14 @@
       <c r="D23">
         <v>-5.172413793103449E-7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F23">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>62</v>
       </c>
@@ -750,8 +898,14 @@
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F24">
+        <v>0.1903474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>116</v>
       </c>
@@ -763,6 +917,12 @@
       </c>
       <c r="D25">
         <v>5.517241379310345E-6</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2.7778200000000001E-5</v>
+      </c>
+      <c r="F25">
+        <v>0.1903474</v>
       </c>
     </row>
   </sheetData>
@@ -772,15 +932,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C38B1B2-9EDD-0949-814D-2CD4BC0F42C1}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -793,8 +953,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -807,8 +973,14 @@
       <c r="D2">
         <v>-4.7765793528505391E-5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F2">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -821,8 +993,14 @@
       <c r="D3">
         <v>4.4684129429892142E-6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F3">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -835,8 +1013,14 @@
       <c r="D4">
         <v>4.0523882896764248E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F4">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -849,8 +1033,14 @@
       <c r="D5">
         <v>8.5208012326656394E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F5">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>30</v>
       </c>
@@ -863,8 +1053,14 @@
       <c r="D6">
         <v>1.7473035439137134E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F6">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>40</v>
       </c>
@@ -877,8 +1073,14 @@
       <c r="D7">
         <v>1.901386748844376E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F7">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>62</v>
       </c>
@@ -891,8 +1093,14 @@
       <c r="D8">
         <v>2.329738058551618E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F8">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>116</v>
       </c>
@@ -905,8 +1113,14 @@
       <c r="D9">
         <v>2.7442218798150999E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F9">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -919,8 +1133,14 @@
       <c r="D10">
         <v>-3.1641791044776114E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F10">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -933,8 +1153,14 @@
       <c r="D11">
         <v>6.8064516129032258E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F11">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -947,8 +1173,14 @@
       <c r="D12">
         <v>1.432258064516129E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F12">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>8</v>
       </c>
@@ -961,8 +1193,14 @@
       <c r="D13">
         <v>3.1709677419354835E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F13">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>30</v>
       </c>
@@ -975,8 +1213,14 @@
       <c r="D14">
         <v>3.4258064516129032E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>40</v>
       </c>
@@ -989,8 +1233,14 @@
       <c r="D15">
         <v>5.912903225806451E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F15">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>62</v>
       </c>
@@ -1003,8 +1253,14 @@
       <c r="D16">
         <v>7.645161290322581E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F16">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>116</v>
       </c>
@@ -1017,8 +1273,14 @@
       <c r="D17">
         <v>9.0645161290322574E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F17">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1031,8 +1293,14 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F18">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1045,8 +1313,14 @@
       <c r="D19">
         <v>4.4979919678714854E-5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F19">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1059,8 +1333,14 @@
       <c r="D20">
         <v>8.2128514056224898E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F20">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1073,8 +1353,14 @@
       <c r="D21">
         <v>2.016064257028112E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F21">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1087,8 +1373,14 @@
       <c r="D22">
         <v>3.2650602409638554E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F22">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>40</v>
       </c>
@@ -1101,8 +1393,14 @@
       <c r="D23">
         <v>3.6546184738955818E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F23">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>62</v>
       </c>
@@ -1115,8 +1413,14 @@
       <c r="D24">
         <v>3.8232931726907629E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F24">
+        <v>0.35365289999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>116</v>
       </c>
@@ -1128,6 +1432,12 @@
       </c>
       <c r="D25">
         <v>4.1285140562248996E-4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.6545170000000003E-5</v>
+      </c>
+      <c r="F25">
+        <v>0.35365289999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1137,15 +1447,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4C9BE1-B9C5-4A4F-99D4-38A4A68F1029}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1158,8 +1468,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1172,8 +1488,14 @@
       <c r="D2">
         <v>1.0222222222222222E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F2">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1186,8 +1508,14 @@
       <c r="D3">
         <v>4.3333333333333334E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F3">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1200,8 +1528,14 @@
       <c r="D4">
         <v>-1.2777777777777777E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F4">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1214,8 +1548,14 @@
       <c r="D5">
         <v>-2.0555555555555555E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F5">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>30</v>
       </c>
@@ -1228,8 +1568,14 @@
       <c r="D6">
         <v>1.3833333333333333E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F6">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>40</v>
       </c>
@@ -1242,8 +1588,14 @@
       <c r="D7">
         <v>5.8888888888888889E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F7">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>62</v>
       </c>
@@ -1256,8 +1608,14 @@
       <c r="D8">
         <v>8.7777777777777767E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F8">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>116</v>
       </c>
@@ -1270,8 +1628,14 @@
       <c r="D9">
         <v>1.7777777777777779E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F9">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1284,8 +1648,14 @@
       <c r="D10">
         <v>-4.8000000000000001E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F10">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1298,8 +1668,14 @@
       <c r="D11">
         <v>-1.7E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F11">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1312,8 +1688,14 @@
       <c r="D12">
         <v>8.4999999999999999E-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F12">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1326,8 +1708,14 @@
       <c r="D13">
         <v>2.9E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F13">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>30</v>
       </c>
@@ -1340,8 +1728,14 @@
       <c r="D14">
         <v>3.6999999999999998E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>40</v>
       </c>
@@ -1354,8 +1748,14 @@
       <c r="D15">
         <v>3.8500000000000001E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F15">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>62</v>
       </c>
@@ -1368,8 +1768,14 @@
       <c r="D16">
         <v>5.9500000000000003E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F16">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>116</v>
       </c>
@@ -1382,8 +1788,14 @@
       <c r="D17">
         <v>-2.9E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F17">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1396,8 +1808,14 @@
       <c r="D18">
         <v>-4.9999999999999996E-6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F18">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1410,8 +1828,14 @@
       <c r="D19">
         <v>-8.1818181818181813E-6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F19">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1424,8 +1848,14 @@
       <c r="D20">
         <v>2.2727272727272728E-6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F20">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1438,8 +1868,14 @@
       <c r="D21">
         <v>1.1818181818181817E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F21">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1452,8 +1888,14 @@
       <c r="D22">
         <v>2.8636363636363634E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F22">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>40</v>
       </c>
@@ -1466,8 +1908,14 @@
       <c r="D23">
         <v>6.6818181818181817E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F23">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>62</v>
       </c>
@@ -1480,8 +1928,14 @@
       <c r="D24">
         <v>1.0909090909090908E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F24">
+        <v>0.1622585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>116</v>
       </c>
@@ -1493,6 +1947,12 @@
       </c>
       <c r="D25">
         <v>1.6318181818181818E-4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.0206049999999997E-5</v>
+      </c>
+      <c r="F25">
+        <v>0.1622585</v>
       </c>
     </row>
   </sheetData>
@@ -1502,15 +1962,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBABDD5-02BD-7842-9670-0AF2AD14992F}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1523,8 +1983,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1537,8 +2003,14 @@
       <c r="D2">
         <v>-5.5462184873949589E-5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F2">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1551,8 +2023,14 @@
       <c r="D3">
         <v>-2.0168067226890759E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F3">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1565,8 +2043,14 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F4">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1579,8 +2063,14 @@
       <c r="D5">
         <v>-7.5630252100840342E-6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F5">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>30</v>
       </c>
@@ -1593,8 +2083,14 @@
       <c r="D6">
         <v>4.1596638655462187E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F6">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>40</v>
       </c>
@@ -1607,8 +2103,14 @@
       <c r="D7">
         <v>3.4453781512605041E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F7">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>62</v>
       </c>
@@ -1621,8 +2123,14 @@
       <c r="D8">
         <v>1.6806722689075631E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F8">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>116</v>
       </c>
@@ -1635,8 +2143,14 @@
       <c r="D9">
         <v>7.8571428571428566E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F9">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1649,8 +2163,14 @@
       <c r="D10">
         <v>1.2653061224489795E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F10">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1663,8 +2183,14 @@
       <c r="D11">
         <v>3.7142857142857143E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F11">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1677,8 +2203,14 @@
       <c r="D12">
         <v>3.3877551020408163E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F12">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1691,8 +2223,14 @@
       <c r="D13">
         <v>1.183673469387755E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F13">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>30</v>
       </c>
@@ -1705,8 +2243,14 @@
       <c r="D14">
         <v>2.6938775510204081E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>40</v>
       </c>
@@ -1719,8 +2263,14 @@
       <c r="D15">
         <v>6.1632653061224492E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F15">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>62</v>
       </c>
@@ -1733,8 +2283,14 @@
       <c r="D16">
         <v>8.2857142857142846E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F16">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>116</v>
       </c>
@@ -1747,8 +2303,14 @@
       <c r="D17">
         <v>2.3265306122448976E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F17">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1761,8 +2323,14 @@
       <c r="D18">
         <v>-9.5833333333333336E-6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1775,8 +2343,14 @@
       <c r="D19">
         <v>3.7500000000000001E-6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1789,8 +2363,14 @@
       <c r="D20">
         <v>1.1250000000000001E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1803,8 +2383,14 @@
       <c r="D21">
         <v>2.0416666666666667E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1817,8 +2403,14 @@
       <c r="D22">
         <v>4.0833333333333334E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>40</v>
       </c>
@@ -1831,8 +2423,14 @@
       <c r="D23">
         <v>2.0833333333333336E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F23">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>62</v>
       </c>
@@ -1845,8 +2443,14 @@
       <c r="D24">
         <v>5.2500000000000002E-5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F24">
+        <v>0.18870200000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>116</v>
       </c>
@@ -1858,6 +2462,12 @@
       </c>
       <c r="D25">
         <v>9.333333333333333E-5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.2189340000000001E-5</v>
+      </c>
+      <c r="F25">
+        <v>0.18870200000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1868,15 +2478,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF963284-84A1-8E45-B660-28A854D065DE}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1889,8 +2499,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1903,8 +2519,14 @@
       <c r="D2">
         <v>-7.2727272727272715E-6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F2">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1917,8 +2539,14 @@
       <c r="D3">
         <v>-2.1363636363636362E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F3">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1931,8 +2559,14 @@
       <c r="D4">
         <v>-1.6363636363636363E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F4">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1945,8 +2579,14 @@
       <c r="D5">
         <v>-1.4090909090909091E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F5">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>30</v>
       </c>
@@ -1959,8 +2599,14 @@
       <c r="D6">
         <v>2.9545454545454542E-6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F6">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>40</v>
       </c>
@@ -1973,8 +2619,14 @@
       <c r="D7">
         <v>1.8863636363636362E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F7">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>62</v>
       </c>
@@ -1987,8 +2639,14 @@
       <c r="D8">
         <v>2.8636363636363634E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F8">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>116</v>
       </c>
@@ -2001,8 +2659,14 @@
       <c r="D9">
         <v>4.568181818181818E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F9">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2015,8 +2679,14 @@
       <c r="D10">
         <v>-9.4736842105263172E-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F10">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2029,8 +2699,14 @@
       <c r="D11">
         <v>-1.0526315789473683E-6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F11">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2043,8 +2719,14 @@
       <c r="D12">
         <v>-1.2631578947368422E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F12">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2057,8 +2739,14 @@
       <c r="D13">
         <v>-3.1578947368421056E-6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F13">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>30</v>
       </c>
@@ -2071,8 +2759,14 @@
       <c r="D14">
         <v>4.1052631578947371E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>40</v>
       </c>
@@ -2085,8 +2779,14 @@
       <c r="D15">
         <v>4.2631578947368425E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F15">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>62</v>
       </c>
@@ -2099,8 +2799,14 @@
       <c r="D16">
         <v>6.3157894736842103E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F16">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>116</v>
       </c>
@@ -2113,8 +2819,14 @@
       <c r="D17">
         <v>9.2631578947368427E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F17">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2127,8 +2839,14 @@
       <c r="D18">
         <v>-6.2608695652173921E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F18">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2141,8 +2859,14 @@
       <c r="D19">
         <v>-2.4782608695652179E-5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F19">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2155,8 +2879,14 @@
       <c r="D20">
         <v>-4.1739130434782612E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F20">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2169,8 +2899,14 @@
       <c r="D21">
         <v>-8.2608695652173923E-6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F21">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>30</v>
       </c>
@@ -2183,8 +2919,14 @@
       <c r="D22">
         <v>3.6086956521739134E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F22">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>40</v>
       </c>
@@ -2197,8 +2939,14 @@
       <c r="D23">
         <v>3.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F23">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>62</v>
       </c>
@@ -2211,8 +2959,14 @@
       <c r="D24">
         <v>8.3478260869565224E-5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F24">
+        <v>0.19342699999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>116</v>
       </c>
@@ -2224,6 +2978,12 @@
       </c>
       <c r="D25">
         <v>1.5782608695652175E-4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4.529482E-5</v>
+      </c>
+      <c r="F25">
+        <v>0.19342699999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>